<commit_message>
All the pages of login and enterpage and driver manager except task page
</commit_message>
<xml_diff>
--- a/src/test/resources/acti/testdata/Actitimedata.xlsx
+++ b/src/test/resources/acti/testdata/Actitimedata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prash\git\actitimeAutomation18\src\test\resources\acti\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC83DED-F8E4-4CF1-B87E-8853F10BE1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B6B1F8-1627-4F5D-9FE2-10D90FE2BFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>admin</t>
   </si>
@@ -348,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -364,22 +364,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>